<commit_message>
Reworked style-setting for pupil-course tables.
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Schuldaten/Fachbelegung/Kurse_10.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Schuldaten/Fachbelegung/Kurse_10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="87">
   <si>
     <t xml:space="preserve">Kursbelegung (Fach+Schüler -&gt; Lehrer)</t>
   </si>
@@ -514,8 +514,12 @@
   </sheetPr>
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X10" activeCellId="0" sqref="X10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1111,9 +1115,7 @@
       <c r="J12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="K12" s="8"/>
       <c r="L12" s="8" t="s">
         <v>59</v>
       </c>
@@ -1186,9 +1188,7 @@
       <c r="J13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="K13" s="8"/>
       <c r="L13" s="8" t="s">
         <v>59</v>
       </c>
@@ -1261,9 +1261,7 @@
       <c r="J14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="K14" s="8"/>
       <c r="L14" s="8" t="s">
         <v>59</v>
       </c>
@@ -1336,9 +1334,7 @@
       <c r="J15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="K15" s="8"/>
       <c r="L15" s="8" t="s">
         <v>59</v>
       </c>

</xml_diff>